<commit_message>
Added parameters | Changed wait stim duration to 3/4 refrate
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/tests/passed_tests_9Mar2021.xlsx
+++ b/experiment/RUN_ME/tests/passed_tests_9Mar2021.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDA3821-89C4-4D4F-837E-72EE820E826C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="151">
   <si>
     <t>Trials in each condition:</t>
   </si>
@@ -454,9 +453,6 @@
     <t>10 No response on recog: make sure you get categor traj and PAS</t>
   </si>
   <si>
-    <t>Ran after fixed timing - changed globals to function inputs</t>
-  </si>
-  <si>
     <t>Checked by tests.m</t>
   </si>
   <si>
@@ -473,12 +469,21 @@
   </si>
   <si>
     <t>checked by photodiodeTest.m</t>
+  </si>
+  <si>
+    <t>Ran after fixed timing - changed globals to function inputs - sub1007.csv</t>
+  </si>
+  <si>
+    <t>there was an error in fixOutput before experiment ended completely</t>
+  </si>
+  <si>
+    <t>I used keypad so number weren't coded correctly.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -638,14 +643,8 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -661,9 +660,6 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -692,6 +688,15 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,8 +705,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FF00FF00"/>
       <color rgb="FF008E40"/>
-      <color rgb="FF00FF00"/>
       <color rgb="FFCCFFFF"/>
     </mruColors>
   </colors>
@@ -714,6 +719,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2029559</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>1060941</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191501" y="20552020"/>
+          <a:ext cx="2029558" cy="1060940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -792,23 +840,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -844,23 +875,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1036,12 +1050,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A116" sqref="A116"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,45 +1080,45 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
+      <c r="A2" s="39" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="32" t="s">
-        <v>143</v>
+      <c r="C4" s="27"/>
+      <c r="D4" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="9" t="s">
         <v>113</v>
       </c>
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -1113,16 +1127,16 @@
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
     </row>
-    <row r="7" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
+    <row r="7" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="34">
+      <c r="B7" s="31">
         <v>12</v>
       </c>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32" t="s">
-        <v>143</v>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1164,29 +1178,29 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="41" t="s">
         <v>116</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="40" t="s">
         <v>119</v>
       </c>
       <c r="B14" s="15"/>
@@ -1194,908 +1208,918 @@
       <c r="D14" s="14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="41" t="s">
         <v>110</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="14"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="8"/>
+      <c r="B19" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="8"/>
+      <c r="B24" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="8"/>
+      <c r="B25" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="14"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="29" t="s">
         <v>125</v>
       </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36" t="s">
+      <c r="C28" s="33"/>
+      <c r="D28" s="33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>127</v>
+      </c>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="B29" s="32" t="s">
-        <v>127</v>
-      </c>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="32"/>
+      <c r="B31" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="33"/>
+      <c r="D32" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="32"/>
+      <c r="B33" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="33"/>
+      <c r="D33" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="23" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="B30" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="35"/>
-      <c r="B31" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="36"/>
-      <c r="D32" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="35"/>
-      <c r="B33" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="36"/>
-      <c r="D33" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>147</v>
-      </c>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="24"/>
-      <c r="B35" s="37" t="s">
+      <c r="A35" s="22"/>
+      <c r="B35" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="32" t="s">
-        <v>143</v>
+      <c r="C35" s="21"/>
+      <c r="D35" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="35" t="s">
         <v>12</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="39" t="s">
+      <c r="A37" s="36" t="s">
         <v>121</v>
       </c>
       <c r="B37" s="14"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="32" t="s">
-        <v>143</v>
+      <c r="C37" s="21"/>
+      <c r="D37" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
-      <c r="B40" s="14" t="s">
+      <c r="A40" s="8"/>
+      <c r="B40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="13"/>
       <c r="B41" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="23"/>
-      <c r="D42" s="23"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="13"/>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="23"/>
-      <c r="D43" s="23"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="13"/>
       <c r="B44" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="13"/>
       <c r="B45" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C46" s="23"/>
-      <c r="D46" s="23"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C47" s="23"/>
-      <c r="D47" s="23"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="13"/>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="13"/>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C50" s="23"/>
-      <c r="D50" s="23"/>
+      <c r="C50" s="21"/>
+      <c r="D50" s="21"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
-      <c r="B51" s="14" t="s">
+      <c r="A51" s="8"/>
+      <c r="B51" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C51" s="23"/>
-      <c r="D51" s="23"/>
+      <c r="C51" s="21"/>
+      <c r="D51" s="21"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
-      <c r="B52" s="14" t="s">
+      <c r="A52" s="8"/>
+      <c r="B52" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C52" s="23"/>
-      <c r="D52" s="23"/>
+      <c r="C52" s="21"/>
+      <c r="D52" s="21"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="14" t="s">
+      <c r="A53" s="8"/>
+      <c r="B53" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C53" s="23"/>
-      <c r="D53" s="23"/>
+      <c r="C53" s="21"/>
+      <c r="D53" s="21"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C54" s="23"/>
-      <c r="D54" s="23"/>
+      <c r="C54" s="21"/>
+      <c r="D54" s="21"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
-      <c r="B55" s="14" t="s">
+      <c r="A55" s="8"/>
+      <c r="B55" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C55" s="23"/>
-      <c r="D55" s="23"/>
+      <c r="C55" s="21"/>
+      <c r="D55" s="21"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="13"/>
       <c r="B56" s="14"/>
-      <c r="C56" s="23"/>
-      <c r="D56" s="23"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="21"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
+      <c r="A57" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B57" s="18"/>
-      <c r="C57" s="26"/>
-      <c r="D57" s="26"/>
+      <c r="B57" s="17"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="35" t="s">
+      <c r="A58" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="C58" s="23"/>
-      <c r="D58" s="32" t="s">
-        <v>143</v>
+      <c r="C58" s="21"/>
+      <c r="D58" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+      <c r="A59" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="23"/>
-      <c r="D59" s="23"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
-      <c r="B60" s="14" t="s">
+      <c r="A60" s="8"/>
+      <c r="B60" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C60" s="23"/>
-      <c r="D60" s="23"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
-      <c r="B61" s="14" t="s">
+      <c r="A61" s="8"/>
+      <c r="B61" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C61" s="23"/>
-      <c r="D61" s="23"/>
+      <c r="C61" s="21"/>
+      <c r="D61" s="21"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="35" t="s">
+      <c r="A62" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B62" s="31" t="s">
+      <c r="B62" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="C62" s="36"/>
-      <c r="D62" s="32" t="s">
-        <v>143</v>
+      <c r="C62" s="33"/>
+      <c r="D62" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="35"/>
-      <c r="B63" s="31" t="s">
+      <c r="A63" s="32"/>
+      <c r="B63" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="C63" s="36"/>
-      <c r="D63" s="32" t="s">
-        <v>143</v>
+      <c r="C63" s="33"/>
+      <c r="D63" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="35"/>
-      <c r="B64" s="31" t="s">
+      <c r="A64" s="32"/>
+      <c r="B64" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C64" s="36"/>
-      <c r="D64" s="32" t="s">
-        <v>143</v>
+      <c r="C64" s="33"/>
+      <c r="D64" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="35"/>
-      <c r="B65" s="32" t="s">
+      <c r="A65" s="32"/>
+      <c r="B65" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C65" s="36"/>
-      <c r="D65" s="32" t="s">
-        <v>143</v>
+      <c r="C65" s="33"/>
+      <c r="D65" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="35"/>
-      <c r="B66" s="31" t="s">
+      <c r="A66" s="32"/>
+      <c r="B66" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="36"/>
-      <c r="D66" s="32" t="s">
-        <v>143</v>
+      <c r="C66" s="33"/>
+      <c r="D66" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="35"/>
-      <c r="B67" s="31" t="s">
+      <c r="A67" s="32"/>
+      <c r="B67" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C67" s="36"/>
-      <c r="D67" s="32" t="s">
-        <v>143</v>
+      <c r="C67" s="33"/>
+      <c r="D67" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="35"/>
-      <c r="B68" s="31" t="s">
+      <c r="A68" s="32"/>
+      <c r="B68" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="36"/>
-      <c r="D68" s="32" t="s">
-        <v>143</v>
+      <c r="C68" s="33"/>
+      <c r="D68" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="35"/>
-      <c r="B69" s="31" t="s">
+      <c r="A69" s="32"/>
+      <c r="B69" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="36"/>
-      <c r="D69" s="32" t="s">
-        <v>143</v>
+      <c r="C69" s="33"/>
+      <c r="D69" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="35"/>
-      <c r="B70" s="31" t="s">
+      <c r="A70" s="32"/>
+      <c r="B70" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="36"/>
-      <c r="D70" s="32" t="s">
-        <v>143</v>
+      <c r="C70" s="33"/>
+      <c r="D70" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="35"/>
-      <c r="B71" s="31" t="s">
+      <c r="A71" s="32"/>
+      <c r="B71" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="C71" s="36"/>
-      <c r="D71" s="32" t="s">
-        <v>143</v>
+      <c r="C71" s="33"/>
+      <c r="D71" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="35"/>
-      <c r="B72" s="31" t="s">
+      <c r="A72" s="32"/>
+      <c r="B72" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C72" s="36"/>
-      <c r="D72" s="32" t="s">
-        <v>143</v>
+      <c r="C72" s="33"/>
+      <c r="D72" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="35"/>
-      <c r="B73" s="31" t="s">
+      <c r="A73" s="32"/>
+      <c r="B73" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="C73" s="36"/>
-      <c r="D73" s="32" t="s">
-        <v>143</v>
+      <c r="C73" s="33"/>
+      <c r="D73" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="35"/>
-      <c r="B74" s="31" t="s">
+      <c r="A74" s="32"/>
+      <c r="B74" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="36"/>
-      <c r="D74" s="32" t="s">
-        <v>143</v>
+      <c r="C74" s="33"/>
+      <c r="D74" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="35"/>
-      <c r="B75" s="31" t="s">
+      <c r="A75" s="32"/>
+      <c r="B75" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C75" s="36"/>
-      <c r="D75" s="32" t="s">
-        <v>143</v>
+      <c r="C75" s="33"/>
+      <c r="D75" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="35"/>
-      <c r="B76" s="31" t="s">
+      <c r="A76" s="32"/>
+      <c r="B76" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C76" s="36"/>
-      <c r="D76" s="32" t="s">
-        <v>143</v>
+      <c r="C76" s="33"/>
+      <c r="D76" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="35"/>
-      <c r="B77" s="31" t="s">
+      <c r="A77" s="32"/>
+      <c r="B77" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C77" s="36"/>
-      <c r="D77" s="32" t="s">
-        <v>143</v>
+      <c r="C77" s="33"/>
+      <c r="D77" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="35"/>
-      <c r="B78" s="31" t="s">
+      <c r="A78" s="32"/>
+      <c r="B78" s="28" t="s">
         <v>70</v>
       </c>
-      <c r="C78" s="36"/>
-      <c r="D78" s="32" t="s">
-        <v>143</v>
+      <c r="C78" s="33"/>
+      <c r="D78" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="35"/>
-      <c r="B79" s="31" t="s">
+      <c r="A79" s="32"/>
+      <c r="B79" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C79" s="36"/>
-      <c r="D79" s="32" t="s">
-        <v>143</v>
+      <c r="C79" s="33"/>
+      <c r="D79" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="35"/>
-      <c r="B80" s="31" t="s">
+      <c r="A80" s="32"/>
+      <c r="B80" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C80" s="36"/>
-      <c r="D80" s="32" t="s">
-        <v>143</v>
+      <c r="C80" s="33"/>
+      <c r="D80" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="35"/>
-      <c r="B81" s="31" t="s">
+      <c r="A81" s="32"/>
+      <c r="B81" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C81" s="36"/>
-      <c r="D81" s="32" t="s">
-        <v>143</v>
+      <c r="C81" s="33"/>
+      <c r="D81" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="35"/>
-      <c r="B82" s="31" t="s">
+      <c r="A82" s="32"/>
+      <c r="B82" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="C82" s="36"/>
-      <c r="D82" s="32" t="s">
-        <v>143</v>
+      <c r="C82" s="33"/>
+      <c r="D82" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="35"/>
-      <c r="B83" s="31" t="s">
+      <c r="A83" s="32"/>
+      <c r="B83" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C83" s="36"/>
-      <c r="D83" s="32" t="s">
-        <v>143</v>
+      <c r="C83" s="33"/>
+      <c r="D83" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="35"/>
-      <c r="B84" s="31" t="s">
+      <c r="A84" s="32"/>
+      <c r="B84" s="28" t="s">
         <v>76</v>
       </c>
-      <c r="C84" s="36"/>
-      <c r="D84" s="32" t="s">
-        <v>143</v>
+      <c r="C84" s="33"/>
+      <c r="D84" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="35"/>
-      <c r="B85" s="31" t="s">
+      <c r="A85" s="32"/>
+      <c r="B85" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="C85" s="36"/>
-      <c r="D85" s="32" t="s">
-        <v>143</v>
+      <c r="C85" s="33"/>
+      <c r="D85" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="35"/>
-      <c r="B86" s="31" t="s">
+      <c r="A86" s="32"/>
+      <c r="B86" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C86" s="36"/>
-      <c r="D86" s="32" t="s">
-        <v>143</v>
+      <c r="C86" s="33"/>
+      <c r="D86" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="35"/>
-      <c r="B87" s="31" t="s">
+      <c r="A87" s="32"/>
+      <c r="B87" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="C87" s="36"/>
-      <c r="D87" s="32" t="s">
-        <v>143</v>
+      <c r="C87" s="33"/>
+      <c r="D87" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="35"/>
-      <c r="B88" s="31" t="s">
+      <c r="A88" s="32"/>
+      <c r="B88" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="C88" s="36"/>
-      <c r="D88" s="32" t="s">
-        <v>143</v>
+      <c r="C88" s="33"/>
+      <c r="D88" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="35"/>
-      <c r="B89" s="31" t="s">
+      <c r="A89" s="32"/>
+      <c r="B89" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C89" s="36"/>
-      <c r="D89" s="32" t="s">
-        <v>143</v>
+      <c r="C89" s="33"/>
+      <c r="D89" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="35"/>
-      <c r="B90" s="31" t="s">
+      <c r="A90" s="32"/>
+      <c r="B90" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C90" s="36"/>
-      <c r="D90" s="32" t="s">
-        <v>143</v>
+      <c r="C90" s="33"/>
+      <c r="D90" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="35"/>
-      <c r="B91" s="31" t="s">
+      <c r="A91" s="32"/>
+      <c r="B91" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C91" s="36"/>
-      <c r="D91" s="32" t="s">
-        <v>143</v>
+      <c r="C91" s="33"/>
+      <c r="D91" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="35"/>
-      <c r="B92" s="31" t="s">
+      <c r="A92" s="32"/>
+      <c r="B92" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C92" s="36"/>
-      <c r="D92" s="32" t="s">
-        <v>143</v>
+      <c r="C92" s="33"/>
+      <c r="D92" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="35"/>
-      <c r="B93" s="31" t="s">
+      <c r="A93" s="32"/>
+      <c r="B93" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C93" s="36"/>
-      <c r="D93" s="32" t="s">
-        <v>143</v>
+      <c r="C93" s="33"/>
+      <c r="D93" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="35"/>
-      <c r="B94" s="31" t="s">
+      <c r="A94" s="32"/>
+      <c r="B94" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C94" s="36"/>
-      <c r="D94" s="32" t="s">
-        <v>143</v>
+      <c r="C94" s="33"/>
+      <c r="D94" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="35"/>
-      <c r="B95" s="31" t="s">
+      <c r="A95" s="32"/>
+      <c r="B95" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="C95" s="36"/>
-      <c r="D95" s="32" t="s">
-        <v>143</v>
+      <c r="C95" s="33"/>
+      <c r="D95" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="35"/>
-      <c r="B96" s="31" t="s">
+      <c r="A96" s="32"/>
+      <c r="B96" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C96" s="36"/>
-      <c r="D96" s="32" t="s">
-        <v>143</v>
+      <c r="C96" s="33"/>
+      <c r="D96" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="35"/>
-      <c r="B97" s="31" t="s">
+      <c r="A97" s="32"/>
+      <c r="B97" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C97" s="36"/>
-      <c r="D97" s="32" t="s">
-        <v>143</v>
+      <c r="C97" s="33"/>
+      <c r="D97" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="35"/>
-      <c r="B98" s="31" t="s">
+      <c r="A98" s="32"/>
+      <c r="B98" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C98" s="36"/>
-      <c r="D98" s="32" t="s">
-        <v>143</v>
+      <c r="C98" s="33"/>
+      <c r="D98" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="35"/>
-      <c r="B99" s="31" t="s">
+      <c r="A99" s="32"/>
+      <c r="B99" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C99" s="36"/>
-      <c r="D99" s="32" t="s">
-        <v>143</v>
+      <c r="C99" s="33"/>
+      <c r="D99" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="35"/>
-      <c r="B100" s="31" t="s">
+      <c r="A100" s="32"/>
+      <c r="B100" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C100" s="36"/>
-      <c r="D100" s="32" t="s">
-        <v>143</v>
+      <c r="C100" s="33"/>
+      <c r="D100" s="29" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="35"/>
-      <c r="B101" s="31" t="s">
+      <c r="A101" s="32"/>
+      <c r="B101" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C101" s="36"/>
-      <c r="D101" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="90" x14ac:dyDescent="0.2">
-      <c r="A102" s="27" t="s">
+      <c r="C101" s="33"/>
+      <c r="D101" s="29" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A102" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B102" s="20" t="s">
+      <c r="B102" s="18" t="s">
         <v>115</v>
       </c>
-      <c r="C102" s="23"/>
-      <c r="D102" s="28"/>
+      <c r="C102" s="21"/>
+      <c r="D102" s="29"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="40" t="s">
+      <c r="A103" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="B103" s="41" t="s">
+      <c r="B103" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="C103" s="36" t="s">
+      <c r="C103" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="D103" s="36" t="s">
-        <v>148</v>
+      <c r="D103" s="33" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="13" t="s">
+      <c r="A104" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B104" s="20" t="s">
+      <c r="B104" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="C104" s="23"/>
-      <c r="D104" s="23"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="21"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="13"/>
-      <c r="B105" s="20" t="s">
+      <c r="A105" s="8"/>
+      <c r="B105" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C105" s="23"/>
-      <c r="D105" s="23"/>
+      <c r="C105" s="21"/>
+      <c r="D105" s="21"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="13"/>
-      <c r="B106" s="20" t="s">
+      <c r="A106" s="8"/>
+      <c r="B106" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C106" s="23"/>
-      <c r="D106" s="23"/>
+      <c r="C106" s="21"/>
+      <c r="D106" s="21"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="13"/>
-      <c r="B107" s="20" t="s">
+      <c r="A107" s="8"/>
+      <c r="B107" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="C107" s="23"/>
-      <c r="D107" s="23"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="21"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="17" t="s">
+      <c r="A108" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B108" s="18"/>
-      <c r="C108" s="26"/>
-      <c r="D108" s="26"/>
+      <c r="B108" s="17"/>
+      <c r="C108" s="24"/>
+      <c r="D108" s="24"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="13" t="s">
         <v>100</v>
       </c>
       <c r="B109" s="14"/>
-      <c r="C109" s="23"/>
-      <c r="D109" s="23"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="21"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="13" t="s">
         <v>101</v>
       </c>
       <c r="B110" s="14"/>
-      <c r="C110" s="23"/>
-      <c r="D110" s="23"/>
+      <c r="C110" s="21"/>
+      <c r="D110" s="21"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="13" t="s">
@@ -2104,8 +2128,8 @@
       <c r="B111" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C111" s="23"/>
-      <c r="D111" s="23"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="21"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="13" t="s">
@@ -2114,8 +2138,8 @@
       <c r="B112" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C112" s="23"/>
-      <c r="D112" s="23"/>
+      <c r="C112" s="21"/>
+      <c r="D112" s="21"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
@@ -2124,8 +2148,8 @@
       <c r="B113" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="C113" s="23"/>
-      <c r="D113" s="23"/>
+      <c r="C113" s="21"/>
+      <c r="D113" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2133,5 +2157,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>